<commit_message>
last update for the day
</commit_message>
<xml_diff>
--- a/Organisation.xlsx
+++ b/Organisation.xlsx
@@ -231,12 +231,6 @@
 Graylog</t>
   </si>
   <si>
-    <t>Graylog Clustering
-Implémentation Clustering
-dans Datacenter 
-avec CentOS</t>
-  </si>
-  <si>
     <t>ACL flow vers firewall</t>
   </si>
   <si>
@@ -366,6 +360,13 @@
   </si>
   <si>
     <t>Infra exacte?full duplex ou non des firewalls..</t>
+  </si>
+  <si>
+    <t>Notice PowerEdge
+Graylog Clustering
+Implémentation Clustering
+dans Datacenter 
+avec CentOS</t>
   </si>
 </sst>
 </file>
@@ -405,7 +406,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -427,12 +428,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -760,9 +755,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -772,6 +764,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -781,13 +778,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -805,6 +802,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -820,22 +820,22 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -850,17 +850,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1170,7 +1165,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F27" sqref="F27:I27"/>
     </sheetView>
   </sheetViews>
@@ -1187,10 +1182,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="55"/>
       <c r="C1" s="17" t="s">
         <v>8</v>
       </c>
@@ -1200,12 +1195,12 @@
       <c r="E1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
       <c r="J1" s="18" t="s">
         <v>14</v>
       </c>
@@ -1260,7 +1255,7 @@
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
       <c r="I4" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J4" s="21" t="s">
         <v>29</v>
@@ -1280,7 +1275,7 @@
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
       <c r="I5" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J5" s="21" t="s">
         <v>30</v>
@@ -1293,13 +1288,13 @@
       <c r="B6" s="6">
         <v>43255</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="48" t="s">
+      <c r="E6" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F6" s="11" t="s">
@@ -1308,7 +1303,7 @@
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
       <c r="I6" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J6" s="21" t="s">
         <v>31</v>
@@ -1321,11 +1316,11 @@
       <c r="B7" s="6">
         <v>43256</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
       <c r="F7" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
@@ -1341,9 +1336,9 @@
       <c r="B8" s="6">
         <v>43257</v>
       </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
       <c r="F8" s="28"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
@@ -1362,10 +1357,10 @@
       <c r="C9" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
       <c r="F9" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
@@ -1384,10 +1379,10 @@
       <c r="C10" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
       <c r="F10" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
@@ -1404,8 +1399,8 @@
         <v>43260</v>
       </c>
       <c r="C11" s="10"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
       <c r="F11" s="11" t="s">
         <v>54</v>
       </c>
@@ -1424,8 +1419,8 @@
         <v>43261</v>
       </c>
       <c r="C12" s="10"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="49"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="52"/>
       <c r="F12" s="15"/>
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
@@ -1441,19 +1436,19 @@
       <c r="B13" s="6">
         <v>43262</v>
       </c>
-      <c r="C13" s="56" t="s">
+      <c r="C13" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="56" t="s">
+      <c r="D13" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="49"/>
-      <c r="F13" s="46" t="s">
+      <c r="E13" s="52"/>
+      <c r="F13" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
       <c r="J13" s="19" t="s">
         <v>37</v>
       </c>
@@ -1465,15 +1460,15 @@
       <c r="B14" s="6">
         <v>43263</v>
       </c>
-      <c r="C14" s="50"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="43" t="s">
+      <c r="C14" s="53"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
       <c r="J14" s="19" t="s">
         <v>38</v>
       </c>
@@ -1485,15 +1480,15 @@
       <c r="B15" s="6">
         <v>43264</v>
       </c>
-      <c r="C15" s="48"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="43" t="s">
+      <c r="C15" s="51"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
       <c r="J15" s="19" t="s">
         <v>39</v>
       </c>
@@ -1505,15 +1500,15 @@
       <c r="B16" s="6">
         <v>43265</v>
       </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="43" t="s">
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="44"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="46"/>
       <c r="J16" s="19" t="s">
         <v>40</v>
       </c>
@@ -1525,15 +1520,15 @@
       <c r="B17" s="6">
         <v>43266</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="43" t="s">
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
       <c r="J17" s="19" t="s">
         <v>41</v>
       </c>
@@ -1545,15 +1540,15 @@
       <c r="B18" s="6">
         <v>43267</v>
       </c>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="43" t="s">
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="44"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
       <c r="J18" s="19" t="s">
         <v>52</v>
       </c>
@@ -1565,15 +1560,15 @@
       <c r="B19" s="6">
         <v>43268</v>
       </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="43" t="s">
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
       <c r="J19" s="20" t="s">
         <v>42</v>
       </c>
@@ -1586,18 +1581,18 @@
         <v>43269</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="53" t="s">
-        <v>68</v>
+        <v>71</v>
+      </c>
+      <c r="D20" s="56" t="s">
+        <v>105</v>
       </c>
       <c r="E20" s="8"/>
-      <c r="F20" s="43" t="s">
+      <c r="F20" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="45"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="47"/>
       <c r="J20" s="19" t="s">
         <v>43</v>
       </c>
@@ -1610,16 +1605,16 @@
         <v>43270</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" s="54"/>
+        <v>72</v>
+      </c>
+      <c r="D21" s="57"/>
       <c r="E21" s="8"/>
-      <c r="F21" s="43" t="s">
-        <v>92</v>
-      </c>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="45"/>
+      <c r="F21" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="47"/>
       <c r="J21" s="19" t="s">
         <v>44</v>
       </c>
@@ -1632,14 +1627,14 @@
         <v>43271</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="D22" s="54"/>
+        <v>76</v>
+      </c>
+      <c r="D22" s="57"/>
       <c r="E22" s="8"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="36"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="35"/>
       <c r="J22" s="19" t="s">
         <v>45</v>
       </c>
@@ -1652,16 +1647,16 @@
         <v>43272</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23" s="54"/>
+        <v>78</v>
+      </c>
+      <c r="D23" s="57"/>
       <c r="E23" s="8"/>
-      <c r="F23" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="63"/>
+      <c r="F23" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="50"/>
       <c r="J23" s="19"/>
     </row>
     <row r="24" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1672,18 +1667,18 @@
         <v>43273</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="54"/>
+        <v>80</v>
+      </c>
+      <c r="D24" s="57"/>
       <c r="E24" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="43" t="s">
-        <v>93</v>
-      </c>
-      <c r="G24" s="44"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="45"/>
+      <c r="F24" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="47"/>
       <c r="J24" s="20" t="s">
         <v>46</v>
       </c>
@@ -1696,14 +1691,14 @@
         <v>43274</v>
       </c>
       <c r="C25" s="29"/>
-      <c r="D25" s="54"/>
+      <c r="D25" s="57"/>
       <c r="E25" s="8"/>
-      <c r="F25" s="43" t="s">
-        <v>94</v>
-      </c>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="45"/>
+      <c r="F25" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="47"/>
       <c r="J25" s="19" t="s">
         <v>47</v>
       </c>
@@ -1716,14 +1711,14 @@
         <v>43275</v>
       </c>
       <c r="C26" s="29"/>
-      <c r="D26" s="54"/>
+      <c r="D26" s="57"/>
       <c r="E26" s="8"/>
-      <c r="F26" s="43" t="s">
-        <v>95</v>
-      </c>
-      <c r="G26" s="44"/>
-      <c r="H26" s="44"/>
-      <c r="I26" s="45"/>
+      <c r="F26" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="46"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="47"/>
       <c r="J26" s="19" t="s">
         <v>48</v>
       </c>
@@ -1736,18 +1731,18 @@
         <v>43276</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="D27" s="54"/>
-      <c r="E27" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="F27" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="45"/>
+        <v>82</v>
+      </c>
+      <c r="D27" s="57"/>
+      <c r="E27" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="F27" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="47"/>
       <c r="J27" s="19" t="s">
         <v>49</v>
       </c>
@@ -1760,10 +1755,10 @@
         <v>43277</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="D28" s="54"/>
-      <c r="E28" s="38"/>
+        <v>83</v>
+      </c>
+      <c r="D28" s="57"/>
+      <c r="E28" s="40"/>
       <c r="J28" s="19" t="s">
         <v>50</v>
       </c>
@@ -1775,17 +1770,17 @@
       <c r="B29" s="6">
         <v>43278</v>
       </c>
-      <c r="C29" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="D29" s="54"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="45"/>
+      <c r="C29" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="57"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="47"/>
       <c r="J29" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1795,15 +1790,15 @@
       <c r="B30" s="6">
         <v>43279</v>
       </c>
-      <c r="C30" s="59" t="s">
-        <v>91</v>
-      </c>
-      <c r="D30" s="54"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="45"/>
+      <c r="C30" s="62" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" s="57"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="47"/>
       <c r="J30" s="19" t="s">
         <v>51</v>
       </c>
@@ -1815,17 +1810,17 @@
       <c r="B31" s="6">
         <v>43280</v>
       </c>
-      <c r="C31" s="59"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="46" t="s">
-        <v>97</v>
-      </c>
-      <c r="G31" s="65"/>
-      <c r="H31" s="65"/>
-      <c r="I31" s="66"/>
-      <c r="J31" s="67" t="s">
-        <v>102</v>
+      <c r="C31" s="62"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="G31" s="66"/>
+      <c r="H31" s="66"/>
+      <c r="I31" s="67"/>
+      <c r="J31" s="38" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -1835,17 +1830,17 @@
       <c r="B32" s="6">
         <v>43281</v>
       </c>
-      <c r="C32" s="59"/>
-      <c r="D32" s="54"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="43" t="s">
-        <v>98</v>
-      </c>
-      <c r="G32" s="44"/>
-      <c r="H32" s="44"/>
-      <c r="I32" s="45"/>
-      <c r="J32" s="67" t="s">
-        <v>103</v>
+      <c r="C32" s="62"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="G32" s="46"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="47"/>
+      <c r="J32" s="38" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -1855,17 +1850,17 @@
       <c r="B33" s="6">
         <v>43282</v>
       </c>
-      <c r="C33" s="60"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="43" t="s">
-        <v>99</v>
-      </c>
-      <c r="G33" s="44"/>
-      <c r="H33" s="44"/>
-      <c r="I33" s="45"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="G33" s="46"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="47"/>
       <c r="J33" s="68" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -1875,17 +1870,17 @@
       <c r="B34" s="6">
         <v>43283</v>
       </c>
-      <c r="C34" s="57" t="s">
-        <v>75</v>
-      </c>
-      <c r="D34" s="54"/>
+      <c r="C34" s="60" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="57"/>
       <c r="E34" s="31"/>
-      <c r="F34" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="G34" s="44"/>
-      <c r="H34" s="44"/>
-      <c r="I34" s="45"/>
+      <c r="F34" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="G34" s="46"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="47"/>
       <c r="J34" s="69"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -1895,15 +1890,15 @@
       <c r="B35" s="6">
         <v>43284</v>
       </c>
-      <c r="C35" s="57"/>
-      <c r="D35" s="54"/>
+      <c r="C35" s="60"/>
+      <c r="D35" s="57"/>
       <c r="E35" s="30"/>
-      <c r="F35" s="43" t="s">
-        <v>101</v>
-      </c>
-      <c r="G35" s="44"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="45"/>
+      <c r="F35" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="G35" s="46"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="47"/>
       <c r="J35" s="69"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -1913,13 +1908,13 @@
       <c r="B36" s="6">
         <v>43285</v>
       </c>
-      <c r="C36" s="57"/>
-      <c r="D36" s="54"/>
+      <c r="C36" s="60"/>
+      <c r="D36" s="57"/>
       <c r="E36" s="8"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="44"/>
-      <c r="H36" s="44"/>
-      <c r="I36" s="45"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="46"/>
+      <c r="H36" s="46"/>
+      <c r="I36" s="47"/>
       <c r="J36" s="69"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -1929,14 +1924,14 @@
       <c r="B37" s="6">
         <v>43286</v>
       </c>
-      <c r="C37" s="57"/>
-      <c r="D37" s="54"/>
+      <c r="C37" s="60"/>
+      <c r="D37" s="57"/>
       <c r="E37" s="8"/>
       <c r="F37" s="11"/>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
-      <c r="I37" s="64"/>
-      <c r="J37" s="67"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="38"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
@@ -1945,13 +1940,13 @@
       <c r="B38" s="6">
         <v>43287</v>
       </c>
-      <c r="C38" s="57"/>
-      <c r="D38" s="54"/>
+      <c r="C38" s="60"/>
+      <c r="D38" s="57"/>
       <c r="E38" s="8"/>
       <c r="F38" s="11"/>
       <c r="G38" s="12"/>
       <c r="H38" s="12"/>
-      <c r="I38" s="64"/>
+      <c r="I38" s="37"/>
       <c r="J38" s="19"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -1961,13 +1956,13 @@
       <c r="B39" s="6">
         <v>43288</v>
       </c>
-      <c r="C39" s="57"/>
-      <c r="D39" s="54"/>
+      <c r="C39" s="60"/>
+      <c r="D39" s="57"/>
       <c r="E39" s="8"/>
       <c r="F39" s="11"/>
       <c r="G39" s="12"/>
       <c r="H39" s="12"/>
-      <c r="I39" s="64"/>
+      <c r="I39" s="37"/>
       <c r="J39" s="19"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -1977,13 +1972,13 @@
       <c r="B40" s="6">
         <v>43289</v>
       </c>
-      <c r="C40" s="58"/>
-      <c r="D40" s="55"/>
+      <c r="C40" s="61"/>
+      <c r="D40" s="58"/>
       <c r="E40" s="8"/>
       <c r="F40" s="11"/>
       <c r="G40" s="12"/>
       <c r="H40" s="12"/>
-      <c r="I40" s="64"/>
+      <c r="I40" s="37"/>
       <c r="J40" s="19"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -1993,17 +1988,17 @@
       <c r="B41" s="6">
         <v>43290</v>
       </c>
-      <c r="C41" s="51" t="s">
+      <c r="C41" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="D41" s="37"/>
-      <c r="E41" s="37" t="s">
-        <v>87</v>
+      <c r="D41" s="39"/>
+      <c r="E41" s="39" t="s">
+        <v>86</v>
       </c>
       <c r="F41" s="11"/>
       <c r="G41" s="12"/>
       <c r="H41" s="12"/>
-      <c r="I41" s="64"/>
+      <c r="I41" s="37"/>
       <c r="J41" s="19"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -2013,13 +2008,13 @@
       <c r="B42" s="6">
         <v>43291</v>
       </c>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="38"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="40"/>
       <c r="F42" s="11"/>
       <c r="G42" s="12"/>
       <c r="H42" s="12"/>
-      <c r="I42" s="64"/>
+      <c r="I42" s="37"/>
       <c r="J42" s="19"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2029,13 +2024,13 @@
       <c r="B43" s="6">
         <v>43292</v>
       </c>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="38"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="40"/>
       <c r="F43" s="11"/>
       <c r="G43" s="12"/>
       <c r="H43" s="12"/>
-      <c r="I43" s="64"/>
+      <c r="I43" s="37"/>
       <c r="J43" s="19"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -2045,13 +2040,13 @@
       <c r="B44" s="6">
         <v>43293</v>
       </c>
-      <c r="C44" s="38"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="38"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
       <c r="F44" s="11"/>
       <c r="G44" s="12"/>
       <c r="H44" s="12"/>
-      <c r="I44" s="64"/>
+      <c r="I44" s="37"/>
       <c r="J44" s="19"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2061,13 +2056,13 @@
       <c r="B45" s="6">
         <v>43294</v>
       </c>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
       <c r="F45" s="11"/>
       <c r="G45" s="12"/>
       <c r="H45" s="12"/>
-      <c r="I45" s="64"/>
+      <c r="I45" s="37"/>
       <c r="J45" s="19"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -2077,13 +2072,13 @@
       <c r="B46" s="6">
         <v>43295</v>
       </c>
-      <c r="C46" s="38"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="38"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="40"/>
       <c r="F46" s="11"/>
       <c r="G46" s="12"/>
       <c r="H46" s="12"/>
-      <c r="I46" s="64"/>
+      <c r="I46" s="37"/>
       <c r="J46" s="19"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -2093,13 +2088,13 @@
       <c r="B47" s="6">
         <v>43296</v>
       </c>
-      <c r="C47" s="39"/>
-      <c r="D47" s="39"/>
-      <c r="E47" s="39"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="41"/>
+      <c r="E47" s="41"/>
       <c r="F47" s="11"/>
       <c r="G47" s="12"/>
       <c r="H47" s="12"/>
-      <c r="I47" s="64"/>
+      <c r="I47" s="37"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
@@ -2108,10 +2103,10 @@
       <c r="B48" s="6">
         <v>43297</v>
       </c>
-      <c r="C48" s="51" t="s">
-        <v>88</v>
-      </c>
-      <c r="D48" s="37" t="s">
+      <c r="C48" s="54" t="s">
+        <v>87</v>
+      </c>
+      <c r="D48" s="39" t="s">
         <v>15</v>
       </c>
       <c r="E48" s="8"/>
@@ -2123,8 +2118,8 @@
       <c r="B49" s="6">
         <v>43298</v>
       </c>
-      <c r="C49" s="61"/>
-      <c r="D49" s="38"/>
+      <c r="C49" s="64"/>
+      <c r="D49" s="40"/>
       <c r="E49" s="8"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2134,8 +2129,8 @@
       <c r="B50" s="6">
         <v>43299</v>
       </c>
-      <c r="C50" s="61"/>
-      <c r="D50" s="38"/>
+      <c r="C50" s="64"/>
+      <c r="D50" s="40"/>
       <c r="E50" s="8"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2145,8 +2140,8 @@
       <c r="B51" s="6">
         <v>43300</v>
       </c>
-      <c r="C51" s="61"/>
-      <c r="D51" s="38"/>
+      <c r="C51" s="64"/>
+      <c r="D51" s="40"/>
       <c r="E51" s="8"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2156,8 +2151,8 @@
       <c r="B52" s="6">
         <v>43301</v>
       </c>
-      <c r="C52" s="61"/>
-      <c r="D52" s="38"/>
+      <c r="C52" s="64"/>
+      <c r="D52" s="40"/>
       <c r="E52" s="8"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2167,8 +2162,8 @@
       <c r="B53" s="6">
         <v>43302</v>
       </c>
-      <c r="C53" s="61"/>
-      <c r="D53" s="38"/>
+      <c r="C53" s="64"/>
+      <c r="D53" s="40"/>
       <c r="E53" s="8"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -2178,8 +2173,8 @@
       <c r="B54" s="6">
         <v>43303</v>
       </c>
-      <c r="C54" s="61"/>
-      <c r="D54" s="39"/>
+      <c r="C54" s="64"/>
+      <c r="D54" s="41"/>
       <c r="E54" s="8"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2189,8 +2184,8 @@
       <c r="B55" s="6">
         <v>43304</v>
       </c>
-      <c r="C55" s="61"/>
-      <c r="D55" s="51" t="s">
+      <c r="C55" s="64"/>
+      <c r="D55" s="54" t="s">
         <v>58</v>
       </c>
       <c r="E55" s="8"/>
@@ -2202,8 +2197,8 @@
       <c r="B56" s="6">
         <v>43305</v>
       </c>
-      <c r="C56" s="61"/>
-      <c r="D56" s="38"/>
+      <c r="C56" s="64"/>
+      <c r="D56" s="40"/>
       <c r="E56" s="8"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2213,8 +2208,8 @@
       <c r="B57" s="6">
         <v>43306</v>
       </c>
-      <c r="C57" s="61"/>
-      <c r="D57" s="38"/>
+      <c r="C57" s="64"/>
+      <c r="D57" s="40"/>
       <c r="E57" s="8"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2224,8 +2219,8 @@
       <c r="B58" s="6">
         <v>43307</v>
       </c>
-      <c r="C58" s="61"/>
-      <c r="D58" s="38"/>
+      <c r="C58" s="64"/>
+      <c r="D58" s="40"/>
       <c r="E58" s="8"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2235,8 +2230,8 @@
       <c r="B59" s="6">
         <v>43308</v>
       </c>
-      <c r="C59" s="61"/>
-      <c r="D59" s="38"/>
+      <c r="C59" s="64"/>
+      <c r="D59" s="40"/>
       <c r="E59" s="8"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2246,8 +2241,8 @@
       <c r="B60" s="6">
         <v>43309</v>
       </c>
-      <c r="C60" s="61"/>
-      <c r="D60" s="38"/>
+      <c r="C60" s="64"/>
+      <c r="D60" s="40"/>
       <c r="E60" s="8"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2257,8 +2252,8 @@
       <c r="B61" s="6">
         <v>43310</v>
       </c>
-      <c r="C61" s="61"/>
-      <c r="D61" s="39"/>
+      <c r="C61" s="64"/>
+      <c r="D61" s="41"/>
       <c r="E61" s="8"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2268,10 +2263,10 @@
       <c r="B62" s="6">
         <v>43311</v>
       </c>
-      <c r="C62" s="51" t="s">
-        <v>89</v>
-      </c>
-      <c r="D62" s="51"/>
+      <c r="C62" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="D62" s="54"/>
       <c r="E62" s="8"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2281,8 +2276,8 @@
       <c r="B63" s="6">
         <v>43312</v>
       </c>
-      <c r="C63" s="38"/>
-      <c r="D63" s="38"/>
+      <c r="C63" s="40"/>
+      <c r="D63" s="40"/>
       <c r="E63" s="8"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2292,8 +2287,8 @@
       <c r="B64" s="6">
         <v>43313</v>
       </c>
-      <c r="C64" s="38"/>
-      <c r="D64" s="38"/>
+      <c r="C64" s="40"/>
+      <c r="D64" s="40"/>
       <c r="E64" s="8"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2303,8 +2298,8 @@
       <c r="B65" s="6">
         <v>43314</v>
       </c>
-      <c r="C65" s="38"/>
-      <c r="D65" s="38"/>
+      <c r="C65" s="40"/>
+      <c r="D65" s="40"/>
       <c r="E65" s="8"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2314,8 +2309,8 @@
       <c r="B66" s="6">
         <v>43315</v>
       </c>
-      <c r="C66" s="38"/>
-      <c r="D66" s="38"/>
+      <c r="C66" s="40"/>
+      <c r="D66" s="40"/>
       <c r="E66" s="8"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -2325,8 +2320,8 @@
       <c r="B67" s="6">
         <v>43316</v>
       </c>
-      <c r="C67" s="38"/>
-      <c r="D67" s="38"/>
+      <c r="C67" s="40"/>
+      <c r="D67" s="40"/>
       <c r="E67" s="8"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -2336,8 +2331,8 @@
       <c r="B68" s="6">
         <v>43317</v>
       </c>
-      <c r="C68" s="39"/>
-      <c r="D68" s="39"/>
+      <c r="C68" s="41"/>
+      <c r="D68" s="41"/>
       <c r="E68" s="8"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2347,10 +2342,10 @@
       <c r="B69" s="6">
         <v>43318</v>
       </c>
-      <c r="C69" s="51" t="s">
+      <c r="C69" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="D69" s="51" t="s">
+      <c r="D69" s="54" t="s">
         <v>59</v>
       </c>
       <c r="E69" s="24"/>
@@ -2362,8 +2357,8 @@
       <c r="B70" s="6">
         <v>43319</v>
       </c>
-      <c r="C70" s="61"/>
-      <c r="D70" s="38"/>
+      <c r="C70" s="64"/>
+      <c r="D70" s="40"/>
       <c r="E70" s="23"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2373,8 +2368,8 @@
       <c r="B71" s="6">
         <v>43320</v>
       </c>
-      <c r="C71" s="61"/>
-      <c r="D71" s="38"/>
+      <c r="C71" s="64"/>
+      <c r="D71" s="40"/>
       <c r="E71" s="8"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2384,8 +2379,8 @@
       <c r="B72" s="6">
         <v>43321</v>
       </c>
-      <c r="C72" s="61"/>
-      <c r="D72" s="38"/>
+      <c r="C72" s="64"/>
+      <c r="D72" s="40"/>
       <c r="E72" s="8"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2395,8 +2390,8 @@
       <c r="B73" s="6">
         <v>43322</v>
       </c>
-      <c r="C73" s="61"/>
-      <c r="D73" s="38"/>
+      <c r="C73" s="64"/>
+      <c r="D73" s="40"/>
       <c r="E73" s="8"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2406,8 +2401,8 @@
       <c r="B74" s="6">
         <v>43323</v>
       </c>
-      <c r="C74" s="61"/>
-      <c r="D74" s="38"/>
+      <c r="C74" s="64"/>
+      <c r="D74" s="40"/>
       <c r="E74" s="8"/>
     </row>
     <row r="75" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2417,8 +2412,8 @@
       <c r="B75" s="6">
         <v>43324</v>
       </c>
-      <c r="C75" s="61"/>
-      <c r="D75" s="39"/>
+      <c r="C75" s="64"/>
+      <c r="D75" s="41"/>
       <c r="E75" s="8"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2428,10 +2423,10 @@
       <c r="B76" s="6">
         <v>43325</v>
       </c>
-      <c r="C76" s="61"/>
-      <c r="D76" s="51"/>
-      <c r="E76" s="37" t="s">
-        <v>87</v>
+      <c r="C76" s="64"/>
+      <c r="D76" s="54"/>
+      <c r="E76" s="39" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2441,9 +2436,9 @@
       <c r="B77" s="6">
         <v>43326</v>
       </c>
-      <c r="C77" s="61"/>
-      <c r="D77" s="38"/>
-      <c r="E77" s="38"/>
+      <c r="C77" s="64"/>
+      <c r="D77" s="40"/>
+      <c r="E77" s="40"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
@@ -2452,9 +2447,9 @@
       <c r="B78" s="6">
         <v>43327</v>
       </c>
-      <c r="C78" s="61"/>
-      <c r="D78" s="38"/>
-      <c r="E78" s="38"/>
+      <c r="C78" s="64"/>
+      <c r="D78" s="40"/>
+      <c r="E78" s="40"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
@@ -2463,9 +2458,9 @@
       <c r="B79" s="6">
         <v>43328</v>
       </c>
-      <c r="C79" s="61"/>
-      <c r="D79" s="38"/>
-      <c r="E79" s="38"/>
+      <c r="C79" s="64"/>
+      <c r="D79" s="40"/>
+      <c r="E79" s="40"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
@@ -2474,9 +2469,9 @@
       <c r="B80" s="6">
         <v>43329</v>
       </c>
-      <c r="C80" s="61"/>
-      <c r="D80" s="38"/>
-      <c r="E80" s="38"/>
+      <c r="C80" s="64"/>
+      <c r="D80" s="40"/>
+      <c r="E80" s="40"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
@@ -2485,9 +2480,9 @@
       <c r="B81" s="6">
         <v>43330</v>
       </c>
-      <c r="C81" s="61"/>
-      <c r="D81" s="38"/>
-      <c r="E81" s="38"/>
+      <c r="C81" s="64"/>
+      <c r="D81" s="40"/>
+      <c r="E81" s="40"/>
     </row>
     <row r="82" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
@@ -2496,9 +2491,9 @@
       <c r="B82" s="6">
         <v>43331</v>
       </c>
-      <c r="C82" s="62"/>
-      <c r="D82" s="39"/>
-      <c r="E82" s="39"/>
+      <c r="C82" s="65"/>
+      <c r="D82" s="41"/>
+      <c r="E82" s="41"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
@@ -2507,10 +2502,10 @@
       <c r="B83" s="6">
         <v>43332</v>
       </c>
-      <c r="C83" s="51" t="s">
+      <c r="C83" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="D83" s="51" t="s">
+      <c r="D83" s="54" t="s">
         <v>61</v>
       </c>
       <c r="E83" s="8"/>
@@ -2522,8 +2517,8 @@
       <c r="B84" s="6">
         <v>43333</v>
       </c>
-      <c r="C84" s="38"/>
-      <c r="D84" s="38"/>
+      <c r="C84" s="40"/>
+      <c r="D84" s="40"/>
       <c r="E84" s="8"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -2533,8 +2528,8 @@
       <c r="B85" s="6">
         <v>43334</v>
       </c>
-      <c r="C85" s="38"/>
-      <c r="D85" s="38"/>
+      <c r="C85" s="40"/>
+      <c r="D85" s="40"/>
       <c r="E85" s="8"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -2544,8 +2539,8 @@
       <c r="B86" s="6">
         <v>43335</v>
       </c>
-      <c r="C86" s="38"/>
-      <c r="D86" s="38"/>
+      <c r="C86" s="40"/>
+      <c r="D86" s="40"/>
       <c r="E86" s="8"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -2555,8 +2550,8 @@
       <c r="B87" s="6">
         <v>43336</v>
       </c>
-      <c r="C87" s="38"/>
-      <c r="D87" s="38"/>
+      <c r="C87" s="40"/>
+      <c r="D87" s="40"/>
       <c r="E87" s="8"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -2566,8 +2561,8 @@
       <c r="B88" s="6">
         <v>43337</v>
       </c>
-      <c r="C88" s="38"/>
-      <c r="D88" s="38"/>
+      <c r="C88" s="40"/>
+      <c r="D88" s="40"/>
       <c r="E88" s="8"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -2577,8 +2572,8 @@
       <c r="B89" s="6">
         <v>43338</v>
       </c>
-      <c r="C89" s="39"/>
-      <c r="D89" s="39"/>
+      <c r="C89" s="41"/>
+      <c r="D89" s="41"/>
       <c r="E89" s="8"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -2588,10 +2583,10 @@
       <c r="B90" s="6">
         <v>43339</v>
       </c>
-      <c r="C90" s="37" t="s">
+      <c r="C90" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="D90" s="51" t="s">
+      <c r="D90" s="54" t="s">
         <v>63</v>
       </c>
       <c r="E90" s="8"/>
@@ -2603,8 +2598,8 @@
       <c r="B91" s="6">
         <v>43340</v>
       </c>
-      <c r="C91" s="38"/>
-      <c r="D91" s="38"/>
+      <c r="C91" s="40"/>
+      <c r="D91" s="40"/>
       <c r="E91" s="8"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -2614,8 +2609,8 @@
       <c r="B92" s="6">
         <v>43341</v>
       </c>
-      <c r="C92" s="38"/>
-      <c r="D92" s="38"/>
+      <c r="C92" s="40"/>
+      <c r="D92" s="40"/>
       <c r="E92" s="8"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -2625,8 +2620,8 @@
       <c r="B93" s="6">
         <v>43342</v>
       </c>
-      <c r="C93" s="38"/>
-      <c r="D93" s="38"/>
+      <c r="C93" s="40"/>
+      <c r="D93" s="40"/>
       <c r="E93" s="8"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2636,8 +2631,8 @@
       <c r="B94" s="6">
         <v>43343</v>
       </c>
-      <c r="C94" s="38"/>
-      <c r="D94" s="38"/>
+      <c r="C94" s="40"/>
+      <c r="D94" s="40"/>
       <c r="E94" s="8"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -2647,8 +2642,8 @@
       <c r="B95" s="6">
         <v>43344</v>
       </c>
-      <c r="C95" s="38"/>
-      <c r="D95" s="38"/>
+      <c r="C95" s="40"/>
+      <c r="D95" s="40"/>
       <c r="E95" s="8"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -2658,8 +2653,8 @@
       <c r="B96" s="6">
         <v>43345</v>
       </c>
-      <c r="C96" s="39"/>
-      <c r="D96" s="39"/>
+      <c r="C96" s="41"/>
+      <c r="D96" s="41"/>
       <c r="E96" s="8"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2669,10 +2664,10 @@
       <c r="B97" s="6">
         <v>43346</v>
       </c>
-      <c r="C97" s="37" t="s">
+      <c r="C97" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="D97" s="51" t="s">
+      <c r="D97" s="54" t="s">
         <v>64</v>
       </c>
       <c r="E97" s="8"/>
@@ -2684,8 +2679,8 @@
       <c r="B98" s="6">
         <v>43347</v>
       </c>
-      <c r="C98" s="38"/>
-      <c r="D98" s="38"/>
+      <c r="C98" s="40"/>
+      <c r="D98" s="40"/>
       <c r="E98" s="8"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2695,8 +2690,8 @@
       <c r="B99" s="6">
         <v>43348</v>
       </c>
-      <c r="C99" s="38"/>
-      <c r="D99" s="38"/>
+      <c r="C99" s="40"/>
+      <c r="D99" s="40"/>
       <c r="E99" s="8"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2706,8 +2701,8 @@
       <c r="B100" s="6">
         <v>43349</v>
       </c>
-      <c r="C100" s="38"/>
-      <c r="D100" s="38"/>
+      <c r="C100" s="40"/>
+      <c r="D100" s="40"/>
       <c r="E100" s="8"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2717,8 +2712,8 @@
       <c r="B101" s="6">
         <v>43350</v>
       </c>
-      <c r="C101" s="38"/>
-      <c r="D101" s="38"/>
+      <c r="C101" s="40"/>
+      <c r="D101" s="40"/>
       <c r="E101" s="8"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2728,8 +2723,8 @@
       <c r="B102" s="6">
         <v>43351</v>
       </c>
-      <c r="C102" s="38"/>
-      <c r="D102" s="38"/>
+      <c r="C102" s="40"/>
+      <c r="D102" s="40"/>
       <c r="E102" s="8"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2739,8 +2734,8 @@
       <c r="B103" s="6">
         <v>43352</v>
       </c>
-      <c r="C103" s="39"/>
-      <c r="D103" s="39"/>
+      <c r="C103" s="41"/>
+      <c r="D103" s="41"/>
       <c r="E103" s="8"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -2750,10 +2745,10 @@
       <c r="B104" s="6">
         <v>43353</v>
       </c>
-      <c r="C104" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="D104" s="51" t="s">
+      <c r="C104" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="D104" s="54" t="s">
         <v>66</v>
       </c>
       <c r="E104" s="8"/>
@@ -2765,8 +2760,8 @@
       <c r="B105" s="6">
         <v>43354</v>
       </c>
-      <c r="C105" s="38"/>
-      <c r="D105" s="38"/>
+      <c r="C105" s="40"/>
+      <c r="D105" s="40"/>
       <c r="E105" s="8"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -2776,8 +2771,8 @@
       <c r="B106" s="6">
         <v>43355</v>
       </c>
-      <c r="C106" s="38"/>
-      <c r="D106" s="38"/>
+      <c r="C106" s="40"/>
+      <c r="D106" s="40"/>
       <c r="E106" s="8"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2787,8 +2782,8 @@
       <c r="B107" s="6">
         <v>43356</v>
       </c>
-      <c r="C107" s="38"/>
-      <c r="D107" s="38"/>
+      <c r="C107" s="40"/>
+      <c r="D107" s="40"/>
       <c r="E107" s="8"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -2798,8 +2793,8 @@
       <c r="B108" s="6">
         <v>43357</v>
       </c>
-      <c r="C108" s="38"/>
-      <c r="D108" s="38"/>
+      <c r="C108" s="40"/>
+      <c r="D108" s="40"/>
       <c r="E108" s="8"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -2809,8 +2804,8 @@
       <c r="B109" s="6">
         <v>43358</v>
       </c>
-      <c r="C109" s="38"/>
-      <c r="D109" s="38"/>
+      <c r="C109" s="40"/>
+      <c r="D109" s="40"/>
       <c r="E109" s="8"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -2820,8 +2815,8 @@
       <c r="B110" s="6">
         <v>43359</v>
       </c>
-      <c r="C110" s="38"/>
-      <c r="D110" s="39"/>
+      <c r="C110" s="40"/>
+      <c r="D110" s="41"/>
       <c r="E110" s="8"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -2831,8 +2826,8 @@
       <c r="B111" s="6">
         <v>43360</v>
       </c>
-      <c r="C111" s="38"/>
-      <c r="D111" s="51" t="s">
+      <c r="C111" s="40"/>
+      <c r="D111" s="54" t="s">
         <v>67</v>
       </c>
       <c r="E111" s="8"/>
@@ -2844,8 +2839,8 @@
       <c r="B112" s="6">
         <v>43361</v>
       </c>
-      <c r="C112" s="38"/>
-      <c r="D112" s="38"/>
+      <c r="C112" s="40"/>
+      <c r="D112" s="40"/>
       <c r="E112" s="8"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -2855,8 +2850,8 @@
       <c r="B113" s="6">
         <v>43362</v>
       </c>
-      <c r="C113" s="38"/>
-      <c r="D113" s="38"/>
+      <c r="C113" s="40"/>
+      <c r="D113" s="40"/>
       <c r="E113" s="8"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -2866,8 +2861,8 @@
       <c r="B114" s="6">
         <v>43363</v>
       </c>
-      <c r="C114" s="38"/>
-      <c r="D114" s="38"/>
+      <c r="C114" s="40"/>
+      <c r="D114" s="40"/>
       <c r="E114" s="8"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -2877,8 +2872,8 @@
       <c r="B115" s="6">
         <v>43364</v>
       </c>
-      <c r="C115" s="38"/>
-      <c r="D115" s="38"/>
+      <c r="C115" s="40"/>
+      <c r="D115" s="40"/>
       <c r="E115" s="8"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -2888,8 +2883,8 @@
       <c r="B116" s="6">
         <v>43365</v>
       </c>
-      <c r="C116" s="38"/>
-      <c r="D116" s="38"/>
+      <c r="C116" s="40"/>
+      <c r="D116" s="40"/>
       <c r="E116" s="8"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -2899,8 +2894,8 @@
       <c r="B117" s="6">
         <v>43366</v>
       </c>
-      <c r="C117" s="39"/>
-      <c r="D117" s="39"/>
+      <c r="C117" s="41"/>
+      <c r="D117" s="41"/>
       <c r="E117" s="8"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -2983,77 +2978,77 @@
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="2"/>
-      <c r="C125" s="40" t="s">
-        <v>85</v>
-      </c>
-      <c r="D125" s="41"/>
-      <c r="E125" s="41"/>
+      <c r="C125" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="D125" s="43"/>
+      <c r="E125" s="43"/>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
-      <c r="C126" s="42"/>
-      <c r="D126" s="42"/>
-      <c r="E126" s="42"/>
+      <c r="C126" s="44"/>
+      <c r="D126" s="44"/>
+      <c r="E126" s="44"/>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
-      <c r="C127" s="42"/>
-      <c r="D127" s="42"/>
-      <c r="E127" s="42"/>
+      <c r="C127" s="44"/>
+      <c r="D127" s="44"/>
+      <c r="E127" s="44"/>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
-      <c r="C128" s="42"/>
-      <c r="D128" s="42"/>
-      <c r="E128" s="42"/>
+      <c r="C128" s="44"/>
+      <c r="D128" s="44"/>
+      <c r="E128" s="44"/>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
-      <c r="C129" s="42"/>
-      <c r="D129" s="42"/>
-      <c r="E129" s="42"/>
+      <c r="C129" s="44"/>
+      <c r="D129" s="44"/>
+      <c r="E129" s="44"/>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
-      <c r="C130" s="42"/>
-      <c r="D130" s="42"/>
-      <c r="E130" s="42"/>
+      <c r="C130" s="44"/>
+      <c r="D130" s="44"/>
+      <c r="E130" s="44"/>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
-      <c r="C131" s="42"/>
-      <c r="D131" s="42"/>
-      <c r="E131" s="42"/>
+      <c r="C131" s="44"/>
+      <c r="D131" s="44"/>
+      <c r="E131" s="44"/>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
-      <c r="C132" s="42"/>
-      <c r="D132" s="42"/>
-      <c r="E132" s="42"/>
+      <c r="C132" s="44"/>
+      <c r="D132" s="44"/>
+      <c r="E132" s="44"/>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
-      <c r="C133" s="42"/>
-      <c r="D133" s="42"/>
-      <c r="E133" s="42"/>
+      <c r="C133" s="44"/>
+      <c r="D133" s="44"/>
+      <c r="E133" s="44"/>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
-      <c r="C134" s="42"/>
-      <c r="D134" s="42"/>
-      <c r="E134" s="42"/>
+      <c r="C134" s="44"/>
+      <c r="D134" s="44"/>
+      <c r="E134" s="44"/>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
-      <c r="C135" s="42"/>
-      <c r="D135" s="42"/>
-      <c r="E135" s="42"/>
+      <c r="C135" s="44"/>
+      <c r="D135" s="44"/>
+      <c r="E135" s="44"/>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
-      <c r="C136" s="42"/>
-      <c r="D136" s="42"/>
-      <c r="E136" s="42"/>
+      <c r="C136" s="44"/>
+      <c r="D136" s="44"/>
+      <c r="E136" s="44"/>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
@@ -3398,12 +3393,12 @@
     <mergeCell ref="F34:I34"/>
     <mergeCell ref="F35:I35"/>
     <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F33:I33"/>
     <mergeCell ref="F24:I24"/>
     <mergeCell ref="F25:I25"/>
     <mergeCell ref="F26:I26"/>
     <mergeCell ref="F27:I27"/>
     <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F33:I33"/>
     <mergeCell ref="F29:I29"/>
     <mergeCell ref="F30:I30"/>
     <mergeCell ref="C48:C61"/>

</xml_diff>